<commit_message>
Видео Python Экспорт из Excel в jpg https://youtu.be/dn3Oi7oaMT4
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>https://youtu.be/2ZWYnSryU9c</t>
   </si>
@@ -69,6 +70,18 @@
   </si>
   <si>
     <t>Прочие ссылки</t>
+  </si>
+  <si>
+    <t>Hola!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azzrael Code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YouTube </t>
+  </si>
+  <si>
+    <t>subs</t>
   </si>
 </sst>
 </file>
@@ -434,7 +447,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,4 +525,39 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>